<commit_message>
fout in datum kolom
</commit_message>
<xml_diff>
--- a/Data/Bronze/wedstrijden.xlsx
+++ b/Data/Bronze/wedstrijden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosyn\Desktop\thesis\thesis_code\Data\Bronze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ECD9B9-70FA-4957-872F-391FE2164A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EC2A32-61CD-40C3-88A3-D0575F75D37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{24801A3F-76ED-4046-A14F-1EEB0CB592AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24801A3F-76ED-4046-A14F-1EEB0CB592AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="151">
   <si>
     <t>wedstrijd_id</t>
   </si>
@@ -303,9 +303,6 @@
   </si>
   <si>
     <t>0v10</t>
-  </si>
-  <si>
-    <t>20/09/024</t>
   </si>
   <si>
     <t>n</t>
@@ -867,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EA0682-CE83-406F-BFF2-25684B614964}">
   <dimension ref="A1:F232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="E219" sqref="E219"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -920,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -940,7 +937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -960,7 +957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -980,7 +977,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -997,7 +994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1014,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1031,7 +1028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1048,7 +1045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1068,7 +1065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1088,7 +1085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1108,7 +1105,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1125,7 +1122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1145,7 +1142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1162,7 +1159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1179,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1213,7 +1210,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1233,7 +1230,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1270,7 +1267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1290,7 +1287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1307,7 +1304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1327,7 +1324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1344,7 +1341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1358,7 +1355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1375,7 +1372,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1409,7 +1406,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1426,7 +1423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1443,12 +1440,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>45897</v>
+        <v>45532</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1460,7 +1457,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1480,7 +1477,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1500,7 +1497,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1520,7 +1517,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1540,7 +1537,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1560,7 +1557,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1600,7 +1597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1617,7 +1614,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1634,7 +1631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1648,7 +1645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1665,7 +1662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1679,7 +1676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1693,7 +1690,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1707,7 +1704,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1721,7 +1718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1735,7 +1732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1749,7 +1746,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1763,7 +1760,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1777,7 +1774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1791,7 +1788,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1805,7 +1802,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1819,7 +1816,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1833,7 +1830,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1850,7 +1847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1864,7 +1861,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1878,7 +1875,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1892,7 +1889,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1906,7 +1903,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1920,7 +1917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1940,7 +1937,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1980,7 +1977,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2000,7 +1997,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2020,7 +2017,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2040,7 +2037,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2060,7 +2057,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2080,7 +2077,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2100,7 +2097,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2120,7 +2117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2140,7 +2137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2160,7 +2157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2200,7 +2197,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2220,7 +2217,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2237,7 +2234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2254,7 +2251,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2271,7 +2268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2288,7 +2285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2305,7 +2302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2322,7 +2319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2339,7 +2336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2356,7 +2353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2373,7 +2370,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2387,7 +2384,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2404,7 +2401,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2421,7 +2418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2435,7 +2432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2452,7 +2449,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2469,7 +2466,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2486,7 +2483,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2506,7 +2503,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2523,7 +2520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2537,7 +2534,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2551,7 +2548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2565,7 +2562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2582,7 +2579,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2596,7 +2593,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2613,15 +2610,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1">
+        <v>45555</v>
+      </c>
+      <c r="C101" t="s">
         <v>89</v>
-      </c>
-      <c r="C101" t="s">
-        <v>90</v>
       </c>
       <c r="D101" t="s">
         <v>52</v>
@@ -2630,10 +2627,10 @@
         <v>73</v>
       </c>
       <c r="F101" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2647,7 +2644,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2658,13 +2655,13 @@
         <v>4</v>
       </c>
       <c r="D103" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E103" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2678,7 +2675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2689,10 +2686,10 @@
         <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2706,7 +2703,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2720,7 +2717,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2734,7 +2731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2745,10 +2742,10 @@
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2762,10 +2759,10 @@
         <v>34</v>
       </c>
       <c r="F110" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2779,7 +2776,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2793,7 +2790,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2807,7 +2804,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2818,10 +2815,10 @@
         <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2835,7 +2832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2849,7 +2846,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2863,7 +2860,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2874,13 +2871,13 @@
         <v>3</v>
       </c>
       <c r="D118" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E118" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2891,10 +2888,10 @@
         <v>4</v>
       </c>
       <c r="D119" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2922,7 +2919,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2933,10 +2930,10 @@
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2947,10 +2944,10 @@
         <v>4</v>
       </c>
       <c r="D123" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2964,7 +2961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2972,13 +2969,13 @@
         <v>45541</v>
       </c>
       <c r="C125" t="s">
+        <v>100</v>
+      </c>
+      <c r="D125" t="s">
         <v>101</v>
       </c>
-      <c r="D125" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2992,7 +2989,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3003,10 +3000,10 @@
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3020,7 +3017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3031,10 +3028,10 @@
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3045,10 +3042,10 @@
         <v>4</v>
       </c>
       <c r="D130" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3062,7 +3059,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3076,7 +3073,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3090,7 +3087,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3104,7 +3101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3118,7 +3115,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3129,10 +3126,10 @@
         <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3160,10 +3157,10 @@
         <v>45632</v>
       </c>
       <c r="C138" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D138" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E138" t="s">
         <v>42</v>
@@ -3172,7 +3169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3180,7 +3177,7 @@
         <v>45639</v>
       </c>
       <c r="C139" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D139" t="s">
         <v>34</v>
@@ -3189,10 +3186,10 @@
         <v>61</v>
       </c>
       <c r="F139" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3200,7 +3197,7 @@
         <v>45632</v>
       </c>
       <c r="C140" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D140" t="s">
         <v>11</v>
@@ -3209,10 +3206,10 @@
         <v>7</v>
       </c>
       <c r="F140" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3220,10 +3217,10 @@
         <v>45639</v>
       </c>
       <c r="C141" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D141" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E141" t="s">
         <v>28</v>
@@ -3232,7 +3229,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3240,7 +3237,7 @@
         <v>45301</v>
       </c>
       <c r="C142" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D142" t="s">
         <v>41</v>
@@ -3252,7 +3249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3260,16 +3257,16 @@
         <v>45667</v>
       </c>
       <c r="C143" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D143" t="s">
+        <v>95</v>
+      </c>
+      <c r="F143" t="s">
         <v>96</v>
       </c>
-      <c r="F143" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3286,10 +3283,10 @@
         <v>24</v>
       </c>
       <c r="F144" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3306,10 +3303,10 @@
         <v>15</v>
       </c>
       <c r="F145" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3326,10 +3323,10 @@
         <v>61</v>
       </c>
       <c r="F146" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3346,10 +3343,10 @@
         <v>12</v>
       </c>
       <c r="F147" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3357,7 +3354,7 @@
         <v>45569</v>
       </c>
       <c r="C148" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D148" t="s">
         <v>30</v>
@@ -3369,7 +3366,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3389,7 +3386,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3403,10 +3400,10 @@
         <v>83</v>
       </c>
       <c r="F150" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3423,7 +3420,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3434,16 +3431,16 @@
         <v>1</v>
       </c>
       <c r="D152" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E152" t="s">
         <v>20</v>
       </c>
       <c r="F152" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3460,10 +3457,10 @@
         <v>20</v>
       </c>
       <c r="F153" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3471,7 +3468,7 @@
         <v>45576</v>
       </c>
       <c r="C154" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D154" t="s">
         <v>22</v>
@@ -3480,10 +3477,10 @@
         <v>73</v>
       </c>
       <c r="F154" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3491,7 +3488,7 @@
         <v>45577</v>
       </c>
       <c r="C155" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D155" t="s">
         <v>46</v>
@@ -3500,10 +3497,10 @@
         <v>73</v>
       </c>
       <c r="F155" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3511,7 +3508,7 @@
         <v>45583</v>
       </c>
       <c r="C156" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D156" t="s">
         <v>11</v>
@@ -3520,10 +3517,10 @@
         <v>32</v>
       </c>
       <c r="F156" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3540,7 +3537,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3554,10 +3551,10 @@
         <v>83</v>
       </c>
       <c r="F158" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3574,7 +3571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3591,10 +3588,10 @@
         <v>32</v>
       </c>
       <c r="F160" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3605,16 +3602,16 @@
         <v>4</v>
       </c>
       <c r="D161" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E161" t="s">
         <v>49</v>
       </c>
       <c r="F161" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3631,10 +3628,10 @@
         <v>39</v>
       </c>
       <c r="F162" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3654,7 +3651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3665,7 +3662,7 @@
         <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E164" t="s">
         <v>20</v>
@@ -3674,7 +3671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3694,7 +3691,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3714,7 +3711,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3722,19 +3719,19 @@
         <v>45618</v>
       </c>
       <c r="C167" t="s">
+        <v>123</v>
+      </c>
+      <c r="D167" t="s">
         <v>124</v>
-      </c>
-      <c r="D167" t="s">
-        <v>125</v>
       </c>
       <c r="E167" t="s">
         <v>22</v>
       </c>
       <c r="F167" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3754,7 +3751,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3762,7 +3759,7 @@
         <v>45625</v>
       </c>
       <c r="C169" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D169" t="s">
         <v>51</v>
@@ -3771,10 +3768,10 @@
         <v>49</v>
       </c>
       <c r="F169" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3785,16 +3782,16 @@
         <v>3</v>
       </c>
       <c r="D170" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E170" t="s">
         <v>20</v>
       </c>
       <c r="F170" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3811,10 +3808,10 @@
         <v>12</v>
       </c>
       <c r="F171" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3831,10 +3828,10 @@
         <v>33</v>
       </c>
       <c r="F172" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3851,10 +3848,10 @@
         <v>24</v>
       </c>
       <c r="F173" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3865,7 +3862,7 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E174" t="s">
         <v>49</v>
@@ -3874,7 +3871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3894,7 +3891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3905,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E176" t="s">
         <v>20</v>
@@ -3914,7 +3911,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3934,7 +3931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3945,7 +3942,7 @@
         <v>4</v>
       </c>
       <c r="D178" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E178" t="s">
         <v>12</v>
@@ -3954,7 +3951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3965,7 +3962,7 @@
         <v>4</v>
       </c>
       <c r="D179" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E179" t="s">
         <v>32</v>
@@ -3974,7 +3971,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3994,7 +3991,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4005,7 +4002,7 @@
         <v>4</v>
       </c>
       <c r="D181" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E181" t="s">
         <v>7</v>
@@ -4014,7 +4011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4034,7 +4031,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4051,10 +4048,10 @@
         <v>61</v>
       </c>
       <c r="F183" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4071,7 +4068,7 @@
         <v>39</v>
       </c>
       <c r="F184" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
@@ -4085,13 +4082,13 @@
         <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E185" t="s">
         <v>73</v>
       </c>
       <c r="F185" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
@@ -4131,7 +4128,7 @@
         <v>48</v>
       </c>
       <c r="F187" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -4145,7 +4142,7 @@
         <v>3</v>
       </c>
       <c r="D188" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E188" t="s">
         <v>42</v>
@@ -4251,7 +4248,7 @@
         <v>73</v>
       </c>
       <c r="F193" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -4291,7 +4288,7 @@
         <v>28</v>
       </c>
       <c r="F195" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
@@ -4305,13 +4302,13 @@
         <v>3</v>
       </c>
       <c r="D196" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E196" t="s">
         <v>7</v>
       </c>
       <c r="F196" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
@@ -4331,7 +4328,7 @@
         <v>42</v>
       </c>
       <c r="F197" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
@@ -4351,7 +4348,7 @@
         <v>48</v>
       </c>
       <c r="F198" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
@@ -4385,13 +4382,13 @@
         <v>3</v>
       </c>
       <c r="D200" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E200" t="s">
         <v>42</v>
       </c>
       <c r="F200" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
@@ -4411,7 +4408,7 @@
         <v>42</v>
       </c>
       <c r="F201" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
@@ -4431,7 +4428,7 @@
         <v>18</v>
       </c>
       <c r="F202" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
@@ -4451,7 +4448,7 @@
         <v>73</v>
       </c>
       <c r="F203" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -4471,7 +4468,7 @@
         <v>61</v>
       </c>
       <c r="F204" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
@@ -4491,7 +4488,7 @@
         <v>28</v>
       </c>
       <c r="F205" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
@@ -4511,7 +4508,7 @@
         <v>48</v>
       </c>
       <c r="F206" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
@@ -4531,7 +4528,7 @@
         <v>42</v>
       </c>
       <c r="F207" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
@@ -4545,13 +4542,13 @@
         <v>3</v>
       </c>
       <c r="D208" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E208" t="s">
         <v>39</v>
       </c>
       <c r="F208" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -4571,7 +4568,7 @@
         <v>22</v>
       </c>
       <c r="F209" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
@@ -4585,13 +4582,13 @@
         <v>2</v>
       </c>
       <c r="D210" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E210" t="s">
         <v>48</v>
       </c>
       <c r="F210" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
@@ -4631,7 +4628,7 @@
         <v>7</v>
       </c>
       <c r="F212" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.3">
@@ -4651,7 +4648,7 @@
         <v>22</v>
       </c>
       <c r="F213" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.3">
@@ -4671,7 +4668,7 @@
         <v>22</v>
       </c>
       <c r="F214" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.3">
@@ -4702,10 +4699,10 @@
         <v>45758</v>
       </c>
       <c r="C216" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D216" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F216" t="s">
         <v>42</v>
@@ -4719,10 +4716,10 @@
         <v>45751</v>
       </c>
       <c r="C217" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D217" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E217" t="s">
         <v>24</v>
@@ -4736,10 +4733,10 @@
         <v>45751</v>
       </c>
       <c r="C218" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D218" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.3">
@@ -4750,7 +4747,7 @@
         <v>45745</v>
       </c>
       <c r="C219" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D219" t="s">
         <v>56</v>
@@ -4767,10 +4764,10 @@
         <v>45730</v>
       </c>
       <c r="C220" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D220" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F220" t="s">
         <v>8</v>
@@ -4784,10 +4781,10 @@
         <v>45569</v>
       </c>
       <c r="C221" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D221" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F221" t="s">
         <v>73</v>
@@ -4801,13 +4798,13 @@
         <v>45695</v>
       </c>
       <c r="C222" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D222" t="s">
         <v>31</v>
       </c>
       <c r="F222" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.3">
@@ -4818,7 +4815,7 @@
         <v>45604</v>
       </c>
       <c r="C223" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D223" t="s">
         <v>21</v>
@@ -4835,13 +4832,13 @@
         <v>45709</v>
       </c>
       <c r="C224" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D224" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F224" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.3">
@@ -4852,10 +4849,10 @@
         <v>45737</v>
       </c>
       <c r="C225" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D225" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F225" t="s">
         <v>30</v>
@@ -4869,7 +4866,7 @@
         <v>45555</v>
       </c>
       <c r="C226" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D226" t="s">
         <v>51</v>
@@ -4886,13 +4883,13 @@
         <v>45562</v>
       </c>
       <c r="C227" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D227" t="s">
         <v>79</v>
       </c>
       <c r="F227" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.3">
@@ -4903,13 +4900,13 @@
         <v>45583</v>
       </c>
       <c r="C228" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D228" t="s">
         <v>11</v>
       </c>
       <c r="F228" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.3">
@@ -4920,7 +4917,7 @@
         <v>45590</v>
       </c>
       <c r="C229" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D229" t="s">
         <v>75</v>
@@ -4937,7 +4934,7 @@
         <v>45618</v>
       </c>
       <c r="C230" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D230" t="s">
         <v>52</v>
@@ -4954,13 +4951,13 @@
         <v>45625</v>
       </c>
       <c r="C231" t="s">
+        <v>123</v>
+      </c>
+      <c r="D231" t="s">
         <v>124</v>
       </c>
-      <c r="D231" t="s">
-        <v>125</v>
-      </c>
       <c r="F231" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
@@ -4971,7 +4968,7 @@
         <v>45632</v>
       </c>
       <c r="C232" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D232" t="s">
         <v>46</v>
@@ -4986,20 +4983,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="01414313-52fe-41bc-8316-3eb8960f4595" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="01414313-52fe-41bc-8316-3eb8960f4595" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5198,14 +5195,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C66F6A44-84E1-4D0E-848C-100AA9D0D462}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E243CA87-6F74-45AB-BAA2-98934BE561A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5218,6 +5207,14 @@
     <ds:schemaRef ds:uri="01414313-52fe-41bc-8316-3eb8960f4595"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C66F6A44-84E1-4D0E-848C-100AA9D0D462}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>